<commit_message>
Fixed unnecessary ABSA description.
</commit_message>
<xml_diff>
--- a/temp/final_output_ABSA.xlsx
+++ b/temp/final_output_ABSA.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALSL-DEBITS SANLAM      80904421</t>
+          <t>SANLAM      80904421</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -506,7 +506,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALWINDEED   WINDEED D67219 2319J</t>
+          <t>WINDEED   WINDEED D67219 2319J</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALMOMENTUM  DE000669339   6793QL</t>
+          <t>MOMENTUM  DE000669339   6793QL</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -544,7 +544,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALMOMENTUM    099917130   4543AM</t>
+          <t>MOMENTUM    099917130   4543AM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -563,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALMOMENTUM    200727015   5888ZL</t>
+          <t>MOMENTUM    200727015   5888ZL</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -582,7 +582,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALMOMENTUM    314386836   7952CM</t>
+          <t>MOMENTUM    314386836   7952CM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -601,7 +601,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALHOLLARD   HOL6932470    250101</t>
+          <t>HOLLARD   HOL6932470    250101</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -620,7 +620,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALMOMENTUM    099917123   4548AM</t>
+          <t>MOMENTUM    099917123   4548AM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALMOMENTUM    099917117   4556AM</t>
+          <t>MOMENTUM    099917117   4556AM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -658,7 +658,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFEREFT WAGES TV D579 B JAN 2025</t>
+          <t>EFT WAGES TV D579 B JAN 2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -677,7 +677,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFEREFT WAGES ACC D579 B NOV 202</t>
+          <t>EFT WAGES ACC D579 B NOV 202</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -696,7 +696,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ACB DEBIT:EXTERNALWINDEED   WINDEED D67219 2319J</t>
+          <t>WINDEED   WINDEED D67219 2319J</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -734,7 +734,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ACB CREDITCLAIMS    DEB_8509060020080</t>
+          <t>CLAIMS    DEB_8509060020080</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -753,7 +753,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ACB CREDITQNOR001 NORLAND CONS</t>
+          <t>QNOR001 NORLAND CONS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -772,7 +772,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP001 TV D</t>
+          <t>EFT WAGES RVP001 TV D</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -795,7 +795,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP009 TV D</t>
+          <t>EFT WAGES RVP009 TV D</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP010 TV D</t>
+          <t>EFT WAGES RVP010 TV D</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP012 TV D</t>
+          <t>EFT WAGES RVP012 TV D</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -864,7 +864,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP013 TV D</t>
+          <t>EFT WAGES RVP013 TV D</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP021 TV D</t>
+          <t>EFT WAGES RVP021 TV D</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124123 EFT WAGES RVP022 TV D</t>
+          <t>EFT WAGES RVP022 TV D</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ACB CREDITQPHI001</t>
+          <t>QPHI001</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -952,7 +952,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ACB CREDITDCL PREPAID REFUND</t>
+          <t>DCL PREPAID REFUND</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -971,7 +971,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ACB CREDITPAYPROP   DEPOSIT REFUND</t>
+          <t>PAYPROP   DEPOSIT REFUND</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFEREFT WAGES SEEL D583C ACC DEC</t>
+          <t>EFT WAGES SEEL D583C ACC DEC</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFEREFT WAGES SEEL D583C FOOD DE</t>
+          <t>EFT WAGES SEEL D583C FOOD DE</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERBS380000 TRF FROM ABSA CHEQU</t>
+          <t>BS380000 TRF FROM ABSA CHEQU</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERRVP WAG ACCOM JAN2025</t>
+          <t>RVP WAG ACCOM JAN2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERRVP WAGES FOOD JAN2025</t>
+          <t>RVP WAGES FOOD JAN2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1191,7 +1191,11 @@
           <t>BIO PAYMENT TOABSA BANK 720450 DIV9 COCTM</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="D38" t="n">
         <v>300</v>
       </c>
@@ -1276,7 +1280,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124040 EFT WAGE D182</t>
+          <t>EFT WAGE D182</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -1295,7 +1299,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFEREFT WAGE D182 124040</t>
+          <t>EFT WAGE D182 124040</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -1314,7 +1318,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124040 D182 EFT WAGE</t>
+          <t>D182 EFT WAGE</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1333,7 +1337,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFEREFT WAGE D182 124040</t>
+          <t>EFT WAGE D182 124040</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -1352,7 +1356,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124040 D182 EFT WAGE</t>
+          <t>D182 EFT WAGE</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -1371,7 +1375,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ACB CREDITD0568 QUICK STEP</t>
+          <t>D0568 QUICK STEP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -1409,7 +1413,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERD524BEOC14JAN25</t>
+          <t>D524BEOC14JAN25</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -1428,10 +1432,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER720450 DIV9 BUFFALO CITY MM</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
+          <t>DIV9 BUFFALO CITY MM</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="D50" t="n">
         <v>1000</v>
       </c>
@@ -1447,10 +1455,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER720450 DIV9 BUFFALO CITY MM</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
+          <t>DIV9 BUFFALO CITY MM</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="D51" t="n">
         <v>1000</v>
       </c>
@@ -1466,7 +1478,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER532020 D563C EFT WAGE RS MIC</t>
+          <t>D563C EFT WAGE RS MIC</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -1485,7 +1497,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERGARN G DE VOS D535B</t>
+          <t>GARN G DE VOS D535B</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -1504,7 +1516,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERGARN IM TSHABALALA D524B</t>
+          <t>GARN IM TSHABALALA D524B</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -1523,7 +1535,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFER124040 EFT WAGE D182</t>
+          <t>EFT WAGE D182</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -1542,7 +1554,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERABSA PLANT</t>
+          <t>ABSA PLANT</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
@@ -1561,7 +1573,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DEBIT TRANSFERABSA INV TRACKER</t>
+          <t>ABSA INV TRACKER</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>

</xml_diff>